<commit_message>
Better verbiage on template files
Signed-off-by: Rony Xavier <rxavier@mitre.org>
</commit_message>
<xml_diff>
--- a/templates/attestations.template.xlsx
+++ b/templates/attestations.template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rxavier/Documents/CMS/inspec-reporter-json-hdf-master/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rxavier/Documents/CMS/inspec-reporter-json-hdf-master/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EF7CD-9FFB-124E-9302-EECCFC01A5A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ECD511-89FD-CF41-8CA2-3F509526C4D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>Control_ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>test-control-1</t>
   </si>
   <si>
-    <t>Non-expired Status passed</t>
-  </si>
-  <si>
     <t>annually</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>test-control-9</t>
   </si>
   <si>
-    <t>Expired Status passed</t>
-  </si>
-  <si>
     <t>test-control-10</t>
   </si>
   <si>
@@ -122,6 +116,9 @@
   </si>
   <si>
     <t>test-control-16</t>
+  </si>
+  <si>
+    <t>The routine review through interview/examination attests to this control passing</t>
   </si>
 </sst>
 </file>
@@ -969,15 +966,15 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1006,319 +1003,319 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>44292</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
         <v>44292</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>44292</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
         <v>44292</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>44292</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>44292</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
         <v>44292</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
         <v>44292</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
         <v>43744</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1">
         <v>44018</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1">
         <v>44110</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
         <v>44233</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <v>44277</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
         <v>44284</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1">
         <v>44288</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1">
         <v>44290</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>